<commit_message>
Made it to run on local-Test sucessful
</commit_message>
<xml_diff>
--- a/app/src/test/resources/DatasetsforQTrip.xlsx
+++ b/app/src/test/resources/DatasetsforQTrip.xlsx
@@ -348,10 +348,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,7 +399,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1011,12 +1011,12 @@
     <col min="1" max="1" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="24.719285714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="40.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="43.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="46.005" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="35.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>